<commit_message>
add new table named university_program
</commit_message>
<xml_diff>
--- a/program.xlsx
+++ b/program.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="19665" windowHeight="6270"/>
   </bookViews>
   <sheets>
     <sheet name="Lakehead university" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
   <si>
     <t>id</t>
   </si>
   <si>
+    <t>program_english_name</t>
+  </si>
+  <si>
+    <t>program_chinese_name</t>
+  </si>
+  <si>
+    <t>program_category</t>
+  </si>
+  <si>
     <t>MA</t>
   </si>
   <si>
@@ -34,58 +43,423 @@
     <t>TOEFL</t>
   </si>
   <si>
-    <t>program_english_name</t>
-  </si>
-  <si>
-    <t>program_chinese_name</t>
-  </si>
-  <si>
     <t>university_ID</t>
   </si>
   <si>
     <t>university_chinese_name</t>
   </si>
   <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>计算机科学</t>
+  </si>
+  <si>
+    <t>计算机与信息科学</t>
+  </si>
+  <si>
     <t>约克大学</t>
   </si>
   <si>
-    <t>program_category</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
-  </si>
-  <si>
-    <t>计算机科学</t>
-  </si>
-  <si>
-    <t>计算机与信息科学</t>
-  </si>
-  <si>
     <t>湖首大学</t>
+  </si>
+  <si>
+    <t>多伦多大学</t>
+  </si>
+  <si>
+    <t>滑铁卢大学</t>
+  </si>
+  <si>
+    <t>Master of Business Administration</t>
+  </si>
+  <si>
+    <t>工商管理硕士</t>
+  </si>
+  <si>
+    <t>商业、管理与经济</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>物理学</t>
+  </si>
+  <si>
+    <t>科学与应用科学</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -93,26 +467,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="50">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -159,7 +819,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,7 +854,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -402,72 +1062,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="1.28515625" customWidth="1"/>
-    <col min="13" max="13" width="115" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="37.125" customWidth="1"/>
+    <col min="3" max="3" width="22.2833333333333" customWidth="1"/>
+    <col min="4" max="4" width="17.2833333333333" customWidth="1"/>
+    <col min="5" max="6" width="3.375" customWidth="1"/>
+    <col min="7" max="7" width="4.375" customWidth="1"/>
+    <col min="8" max="9" width="6.375" customWidth="1"/>
+    <col min="10" max="10" width="14.875" customWidth="1"/>
+    <col min="11" max="11" width="24.25" customWidth="1"/>
+    <col min="12" max="12" width="1.28333333333333" customWidth="1"/>
+    <col min="13" max="13" width="106.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>9900103001</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -488,26 +1152,26 @@
         <v>9900103</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="M2" t="str">
         <f>CONCATENATE("(",A2,",'",B2,"','",C2,"','",D2,"',",E2,",",F2,",",G2,",",H2,",",I2,",'",J2,"','",K2,"'",")",",")</f>
         <v>(9900103001,'Computer Science','计算机科学','计算机与信息科学',1,1,3.2,6.5,80,'9900103','约克大学'),</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>9900114001</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
       <c r="E3">
         <v>1</v>
       </c>
@@ -515,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H3">
         <v>6.5</v>
@@ -531,11 +1195,402 @@
       </c>
       <c r="M3" t="str">
         <f>CONCATENATE("(",A3,",'",B3,"','",C3,"','",D3,"',",E3,",",F3,",",G3,",",H3,",",I3,",'",J3,"','",K3,"'",")",",")</f>
-        <v>(9900114001,'Computer Science','计算机科学','计算机与信息科学',1,1,3,6.5,78,'9900114','湖首大学'),</v>
+        <v>(9900114001,'Computer Science','计算机科学','计算机与信息科学',1,1,2.5,6.5,78,'9900114','湖首大学'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2">
+        <v>9900101001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3.2</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>85</v>
+      </c>
+      <c r="J4" s="2">
+        <v>9900101</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="str">
+        <f>CONCATENATE("(",A4,",'",B4,"','",C4,"','",D4,"',",E4,",",F4,",",G4,",",H4,",",I4,",'",J4,"','",K4,"'",")",",")</f>
+        <v>(9900101001,'Computer Science','计算机科学','计算机与信息科学',1,1,3.2,7,85,'9900101','多伦多大学'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2">
+        <v>9900102001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9900102</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="str">
+        <f>CONCATENATE("(",A5,",'",B5,"','",C5,"','",D5,"',",E5,",",F5,",",G5,",",H5,",",I5,",'",J5,"','",K5,"'",")",",")</f>
+        <v>(9900102001,'Computer Science','计算机科学','计算机与信息科学',1,1,3,7,80,'9900102','滑铁卢大学'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2">
+        <v>9900103002</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>80</v>
+      </c>
+      <c r="J6" s="2">
+        <v>9900103</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" t="str">
+        <f>CONCATENATE("(",A6,",'",B6,"','",C6,"','",D6,"',",E6,",",F6,",",G6,",",H6,",",I6,",'",J6,"','",K6,"'",")",",")</f>
+        <v>(9900103002,'Master of Business Administration','工商管理硕士','商业、管理与经济',1,0,3.2,6.5,80,'9900103','约克大学'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2">
+        <v>9900114002</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>78</v>
+      </c>
+      <c r="J7" s="2">
+        <v>9900114</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" t="str">
+        <f>CONCATENATE("(",A7,",'",B7,"','",C7,"','",D7,"',",E7,",",F7,",",G7,",",H7,",",I7,",'",J7,"','",K7,"'",")",",")</f>
+        <v>(9900114002,'Master of Business Administration','工商管理硕士','商业、管理与经济',1,0,2.5,6.5,78,'9900114','湖首大学'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2">
+        <v>9900101002</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>90</v>
+      </c>
+      <c r="J8" s="2">
+        <v>9900101</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="str">
+        <f>CONCATENATE("(",A8,",'",B8,"','",C8,"','",D8,"',",E8,",",F8,",",G8,",",H8,",",I8,",'",J8,"','",K8,"'",")",",")</f>
+        <v>(9900101002,'Master of Business Administration','工商管理硕士','商业、管理与经济',1,0,3.2,7.5,90,'9900101','多伦多大学'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2">
+        <v>9900102002</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <v>80</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9900102</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="str">
+        <f>CONCATENATE("(",A9,",'",B9,"','",C9,"','",D9,"',",E9,",",F9,",",G9,",",H9,",",I9,",'",J9,"','",K9,"'",")",",")</f>
+        <v>(9900102002,'Master of Business Administration','工商管理硕士','商业、管理与经济',1,0,3,7,80,'9900102','滑铁卢大学'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2">
+        <v>9900103003</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>80</v>
+      </c>
+      <c r="J10" s="2">
+        <v>9900103</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" t="str">
+        <f>CONCATENATE("(",A10,",'",B10,"','",C10,"','",D10,"',",E10,",",F10,",",G10,",",H10,",",I10,",'",J10,"','",K10,"'",")",",")</f>
+        <v>(9900103003,'Physics','物理学','科学与应用科学',1,1,3,6.5,80,'9900103','约克大学'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2">
+        <v>9900114003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>78</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9900114</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="str">
+        <f>CONCATENATE("(",A11,",'",B11,"','",C11,"','",D11,"',",E11,",",F11,",",G11,",",H11,",",I11,",'",J11,"','",K11,"'",")",",")</f>
+        <v>(9900114003,'Physics','物理学','科学与应用科学',1,1,2.5,6.5,78,'9900114','湖首大学'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2">
+        <v>9900101003</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>85</v>
+      </c>
+      <c r="J12" s="2">
+        <v>9900101</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" t="str">
+        <f>CONCATENATE("(",A12,",'",B12,"','",C12,"','",D12,"',",E12,",",F12,",",G12,",",H12,",",I12,",'",J12,"','",K12,"'",")",",")</f>
+        <v>(9900101003,'Physics','物理学','科学与应用科学',1,1,3.2,6.5,85,'9900101','多伦多大学'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2">
+        <v>9900102003</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="I13" s="2">
+        <v>80</v>
+      </c>
+      <c r="J13" s="2">
+        <v>9900102</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" t="str">
+        <f>CONCATENATE("(",A13,",'",B13,"','",C13,"','",D13,"',",E13,",",F13,",",G13,",",H13,",",I13,",'",J13,"','",K13,"'",")",",")</f>
+        <v>(9900102003,'Physics','物理学','科学与应用科学',1,1,3,6.5,80,'9900102','滑铁卢大学'),</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>